<commit_message>
Änderung der Ordnerstruktur und Erstellung der Datenbank.xlsx
</commit_message>
<xml_diff>
--- a/Medavis_Dispatcher_Lunatec/Data/Config.xlsx
+++ b/Medavis_Dispatcher_Lunatec/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas.jahl\develop\RPA\uipath-rpa_med\Medavis_Dispatcher_Lunatec\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20DA944-6A58-4FBD-90E8-7FE3870A0C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F344D0D4-4579-474D-9367-EA5CC73CD37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36135" yWindow="2520" windowWidth="18150" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -214,13 +214,25 @@
   </si>
   <si>
     <t>rpa004_Working_Folder</t>
+  </si>
+  <si>
+    <t>rpa004_DatenbankOrdner</t>
+  </si>
+  <si>
+    <t>rpa004_InputOrdner</t>
+  </si>
+  <si>
+    <t>rpa004_ErgebnisOrdner</t>
+  </si>
+  <si>
+    <t>rpa004_InputArchivOrdner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -241,6 +253,17 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -265,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -277,6 +300,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -593,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2876,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2997,17 +3022,45 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -3996,5 +4049,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>